<commit_message>
Replaced bmp files with jpg ones
</commit_message>
<xml_diff>
--- a/audit-SEO-chouette.xlsx
+++ b/audit-SEO-chouette.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\excellentia5\Documents\FORMATION\Git-repos\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4A6941-4C5E-4B29-BF85-E17285028594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4932D5F5-9701-420E-9398-43B3BE34F5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>Catégorie</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Seulement des fichiers au format jpg/jpeg ou png</t>
   </si>
   <si>
-    <t>Convertir le fichier img</t>
-  </si>
-  <si>
     <t>Utiliser des animations CSS et afficher un texte en cas d'anomalie</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>Balises meta description manquantes</t>
   </si>
   <si>
-    <t>L'avis laissé par un client est affiché via un fichier img</t>
-  </si>
-  <si>
     <t>Utiliser les validateurs HTML et CSS systématiquement pour vérifier si le code produit respecte les normes</t>
   </si>
   <si>
@@ -247,6 +241,12 @@
   </si>
   <si>
     <t>Modifier la couleur de la police d'écriture ou de l'arrière plan pour favoriser la lecture</t>
+  </si>
+  <si>
+    <t>Convertir les fichiers img</t>
+  </si>
+  <si>
+    <t>Certains textes sont affichés via un fichier img</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -649,13 +649,13 @@
         <v>34</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -663,19 +663,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -695,7 +695,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>20</v>
@@ -735,7 +735,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -755,7 +755,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -792,7 +792,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -800,19 +800,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="G11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -829,7 +829,10 @@
         <v>42</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>43</v>
+        <v>70</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -843,10 +846,10 @@
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -860,27 +863,27 @@
         <v>25</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -888,16 +891,16 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -905,19 +908,19 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="E17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="G17" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Removed texture img files and display
</commit_message>
<xml_diff>
--- a/audit-SEO-chouette.xlsx
+++ b/audit-SEO-chouette.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\excellentia5\Documents\FORMATION\Git-repos\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB7B434-512B-4525-8C38-AB997063E7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B015847D-813B-4B06-9724-83826DB05CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>Catégorie</t>
   </si>
@@ -255,25 +255,40 @@
     <t>Accessibilté (dev)</t>
   </si>
   <si>
-    <t>Défaut de conception du CSS</t>
-  </si>
-  <si>
-    <t>Pour une meilleure maintenabilité du site web, il est préférable d'organiser les éléments dans une flexbox contenue dans une grid</t>
-  </si>
-  <si>
     <t>L'utilisation du CSS rend les mises à jour et maintenances plus chronophages.</t>
   </si>
   <si>
     <t>S'assurer que les versions d'affichage ne présentent pas d'anomalie d'affichage</t>
   </si>
   <si>
-    <t>Implique le rallongement qu'un dev mettra à rechercher les segments à modifier pour mettre à jour ou maintenir le site</t>
-  </si>
-  <si>
     <t>Segmenter le grands fichiers CSS en plusieurs selon la méthode 7-1</t>
   </si>
   <si>
     <t>https://accessibility.belgium.be/fr/articles/images/utilisez-du-vrai-texte-et-pas-du-texte-sous-forme-dimage</t>
+  </si>
+  <si>
+    <t>Défaut de conception du formulaire de contact (CSS)</t>
+  </si>
+  <si>
+    <t>Pour une meilleure maintenabilité du site web, il est préférable d'organiser certains éléments dans une flexbox contenue dans une grid</t>
+  </si>
+  <si>
+    <t>Implique un temps supplémentaire qu'un dev mettra à rechercher les segments à modifier pour mettre à jour ou maintenir le site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                               </t>
+  </si>
+  <si>
+    <t>Les img de textures gènent la lecture des textes</t>
+  </si>
+  <si>
+    <t>Ne pas utiliser d'images de textures ou alors un grain très léger et avec peu d'opacité</t>
+  </si>
+  <si>
+    <t>Les textures trop prononcées peuvent gommer les contrastes entre le texte et l'arrière plan, ce qui peut entrainer des gènes de lectures auprès des utilisateurs</t>
+  </si>
+  <si>
+    <t>Retirer les textures existantes</t>
   </si>
 </sst>
 </file>
@@ -595,11 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -882,116 +897,137 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:26" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1975,6 +2011,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Merged contact.html into index.html
</commit_message>
<xml_diff>
--- a/audit-SEO-chouette.xlsx
+++ b/audit-SEO-chouette.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\excellentia5\Documents\FORMATION\Git-repos\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B015847D-813B-4B06-9724-83826DB05CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BF4358-975F-40E7-B93F-F73DDA5D200F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>Catégorie</t>
   </si>
@@ -150,9 +150,6 @@
     <t>400 mots minimum par page</t>
   </si>
   <si>
-    <t>Rédiger un texte d'au moins 400 mots pour la page2</t>
-  </si>
-  <si>
     <t>Faire pointer les liens externes vers des sites de partenaires officiels</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>Retirer les textures existantes</t>
+  </si>
+  <si>
+    <t>Rédiger un texte d'au moins 400 mots pour la page2 ou fusionner la page contact dans la page accueil</t>
   </si>
 </sst>
 </file>
@@ -333,7 +333,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +349,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -393,6 +399,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -613,8 +622,8 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -649,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -691,13 +700,13 @@
         <v>34</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -705,19 +714,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -737,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -757,7 +766,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -765,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>20</v>
@@ -777,7 +786,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -797,7 +806,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -814,7 +823,10 @@
         <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>85</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -828,13 +840,13 @@
         <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="G10" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -842,19 +854,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="G11" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -868,13 +880,13 @@
         <v>24</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -888,13 +900,13 @@
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -902,19 +914,19 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="G14" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -928,30 +940,31 @@
         <v>25</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -959,22 +972,22 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -982,50 +995,50 @@
         <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="G18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>